<commit_message>
Completed the Authoriization Part and now we are getting Tokens from URL
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Others\webdevbootcamp\spotify-clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C806C7-09EE-4CB0-B010-B87C97A3D9D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663E562B-5E0A-4474-89F0-DFB9149C9F20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Make a Spotify Configuration File which will help us login via a Web API</t>
+  </si>
+  <si>
+    <t>Completed the Authentication Part</t>
+  </si>
+  <si>
+    <t>If user is authorized with Spotify, he gets to see the logged in header else sees the log in page</t>
   </si>
 </sst>
 </file>
@@ -84,11 +90,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -370,64 +381,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.44140625" customWidth="1"/>
-    <col min="2" max="2" width="43.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.5546875" customWidth="1"/>
+    <col min="1" max="1" width="42.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="69.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>44242</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5" s="3">
         <v>44244</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>44245</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Used Context API instead of regular States
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Others\webdevbootcamp\spotify-clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663E562B-5E0A-4474-89F0-DFB9149C9F20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A835A8C8-4661-420C-97C6-5A3C9BE169CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -55,6 +55,33 @@
   </si>
   <si>
     <t>If user is authorized with Spotify, he gets to see the logged in header else sees the log in page</t>
+  </si>
+  <si>
+    <t>Made a Player Page for Spotify Authentication [template only]</t>
+  </si>
+  <si>
+    <t>Read about React Context API</t>
+  </si>
+  <si>
+    <t>Used Context API instead of regular States</t>
+  </si>
+  <si>
+    <t>Passed Spotify as a prop to the Player Component</t>
+  </si>
+  <si>
+    <t>Bypassed the login page by setting the initial value of Token (this step has to be undone later on)</t>
+  </si>
+  <si>
+    <t>Create Player, SideBar, SongRow</t>
+  </si>
+  <si>
+    <t>To Decide</t>
+  </si>
+  <si>
+    <t>Host it on Firebase</t>
+  </si>
+  <si>
+    <t>Share your Spotify Clone App and Knowlegde on Medium</t>
   </si>
 </sst>
 </file>
@@ -381,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,6 +485,67 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>44249</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>44250</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>